<commit_message>
before pulling temp branch code commiting changes
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData/TestData.xlsx
+++ b/src/test/resources/ExcelTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Priyanka Numpy Ninja docs and Projects\LMS_Team15_Apr2024\LMS-Hackathon-Team-15\src\test\resources\ExcelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733AF413-3B3F-4B3C-BD2D-E443CE3F52FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BE8B8C-6451-4F99-BFCC-AEC8FF14B820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="147">
   <si>
     <t>Please login to LMS application</t>
   </si>
@@ -203,9 +203,6 @@
 Login</t>
   </si>
   <si>
-    <t>UpdateUserFirstName</t>
-  </si>
-  <si>
     <t>UpdateUserMiddleName</t>
   </si>
   <si>
@@ -257,15 +254,9 @@
     <t>userComments</t>
   </si>
   <si>
-    <t>Neha</t>
-  </si>
-  <si>
     <t>Nikki</t>
   </si>
   <si>
-    <t>Paul</t>
-  </si>
-  <si>
     <t>New york</t>
   </si>
   <si>
@@ -293,18 +284,6 @@
     <t>UpdateUserComments</t>
   </si>
   <si>
-    <t>Updated User FirstName</t>
-  </si>
-  <si>
-    <t>Updated User MiddleName</t>
-  </si>
-  <si>
-    <t>Updated UserLastName</t>
-  </si>
-  <si>
-    <t>Updated UserLocation</t>
-  </si>
-  <si>
     <t>Updated UserPhoneNo</t>
   </si>
   <si>
@@ -335,9 +314,6 @@
     <t>https://www.linkedin.com/Nikki</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>Inactive</t>
   </si>
   <si>
@@ -353,51 +329,9 @@
     <t>MSC</t>
   </si>
   <si>
-    <t>UpdateMultipleField</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Bhalla</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
-    <t>InvalidUpdatWithExistingPhoneNum</t>
-  </si>
-  <si>
-    <t>InvalidUpdatWithExistingEmail</t>
-  </si>
-  <si>
-    <t>InvalidUpdatWithNonExistingRole</t>
-  </si>
-  <si>
-    <t>InvalidUpdatWithNonExistingRoleStatus</t>
-  </si>
-  <si>
-    <t>InvalidUpdateWithVisaStatus</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>Created</t>
-  </si>
-  <si>
-    <t>DNT</t>
-  </si>
-  <si>
-    <t>VerifyUserDetailsPopup</t>
-  </si>
-  <si>
-    <t>Riya</t>
-  </si>
-  <si>
     <t>Roy</t>
   </si>
   <si>
@@ -407,15 +341,9 @@
     <t>Dallas</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/</t>
-  </si>
-  <si>
     <t>R01</t>
   </si>
   <si>
-    <t>H4 EAD</t>
-  </si>
-  <si>
     <t>BE</t>
   </si>
   <si>
@@ -437,22 +365,112 @@
     <t>Riya@123.com</t>
   </si>
   <si>
-    <t>VerifyUserDetailsPopup1</t>
-  </si>
-  <si>
     <t>RiyaY</t>
   </si>
   <si>
-    <t>RoyY</t>
-  </si>
-  <si>
-    <t>SenN</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/Riya</t>
   </si>
   <si>
     <t>Riya123@mail.com</t>
+  </si>
+  <si>
+    <t>userDetailsPopupText</t>
+  </si>
+  <si>
+    <t>User Details</t>
+  </si>
+  <si>
+    <t>VerifyUserDetailsPopupText</t>
+  </si>
+  <si>
+    <t>UpdateUserAllDetails</t>
+  </si>
+  <si>
+    <t>Riyana</t>
+  </si>
+  <si>
+    <t>Bhatia</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>PST</t>
+  </si>
+  <si>
+    <t>Bcom</t>
+  </si>
+  <si>
+    <t>All user details updated</t>
+  </si>
+  <si>
+    <t>Updated user first name</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>New User for dallas region-updated middle name</t>
+  </si>
+  <si>
+    <t>UpdateMandatoryField</t>
+  </si>
+  <si>
+    <t>H4-EAD</t>
+  </si>
+  <si>
+    <t>InvalidUpdate_NumericValueInLocation</t>
+  </si>
+  <si>
+    <t>InvalidUpdate_ExistingPhoneNum</t>
+  </si>
+  <si>
+    <t>InvalidUpdate_invalidEmail</t>
+  </si>
+  <si>
+    <t>InvalidUpdate_NumericValueInTextField</t>
+  </si>
+  <si>
+    <t>56@12</t>
+  </si>
+  <si>
+    <t>InvalidUpdate_InvalidTimezone</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>123@11</t>
+  </si>
+  <si>
+    <t>UpdateByMissingEmail</t>
+  </si>
+  <si>
+    <t>Updated Timezone</t>
+  </si>
+  <si>
+    <t>UpdateMultipleFields</t>
+  </si>
+  <si>
+    <t>UpdateOptionalFields</t>
+  </si>
+  <si>
+    <t>Bachelors</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>optional fields added</t>
   </si>
 </sst>
 </file>
@@ -482,12 +500,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -503,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -523,8 +547,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1137,385 +1164,1189 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788AA9AD-10DC-4CF5-9D53-5F59AF9B065B}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.77734375" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>71</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1230002345</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="D4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="H4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="O4" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="O5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="9">
+        <v>3033031212</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7">
+        <v>3033031212</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>3033031212</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9">
+        <v>3033031212</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" t="s">
+        <v>94</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10">
+        <v>3033031212</v>
+      </c>
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L10" t="s">
+        <v>95</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11">
+        <v>3033031212</v>
+      </c>
+      <c r="H11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" t="s">
-        <v>78</v>
-      </c>
-      <c r="O7" s="2" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12">
+        <v>3033031212</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" t="s">
+        <v>95</v>
+      </c>
+      <c r="M12" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8">
-        <v>2233445566</v>
-      </c>
-      <c r="O8" s="2" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13">
+        <v>3033031212</v>
+      </c>
+      <c r="H13" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" t="s">
+        <v>99</v>
+      </c>
+      <c r="K13" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M13" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" t="s">
+        <v>98</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="7" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14">
+        <v>3033031212</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" t="s">
+        <v>97</v>
+      </c>
+      <c r="L14" t="s">
+        <v>95</v>
+      </c>
+      <c r="M14" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O14" t="s">
+        <v>98</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15">
+        <v>3033031212</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M15" t="s">
+        <v>96</v>
+      </c>
+      <c r="N15" t="s">
+        <v>124</v>
+      </c>
+      <c r="O15" t="s">
+        <v>98</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="E16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="F16" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3021302111</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" t="s">
+        <v>125</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="G17" s="2">
+        <v>3021302111</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="7" t="s">
+      <c r="J17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="M17" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="P17" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="2">
+        <v>11111</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="2">
+        <v>11111</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="2">
+        <v>11111</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="8">
+        <v>9899</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2890</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" s="2">
+        <v>990011</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23">
+        <v>3033031212</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24">
+        <v>3033031212</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N15" t="s">
-        <v>106</v>
-      </c>
-      <c r="O15" s="2" t="s">
+      <c r="L24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M24" s="7"/>
+      <c r="N24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O24" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F19">
-        <v>2233445566</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="P24" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M25" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="K20" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L23" t="s">
-        <v>119</v>
+      <c r="N25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{1593747E-9B59-4700-95CA-6CF0E43A7512}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{E47A9AAB-4919-4153-BF15-EB8591232BF0}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{02F9C97E-DD15-45D0-B887-FEF05E1DF2EF}"/>
+    <hyperlink ref="M16" r:id="rId1" xr:uid="{1593747E-9B59-4700-95CA-6CF0E43A7512}"/>
+    <hyperlink ref="M17" r:id="rId2" xr:uid="{D95BE6CA-AE57-475B-802E-5E7F1D4CB14F}"/>
+    <hyperlink ref="M3" r:id="rId3" xr:uid="{EBC9CEE7-19ED-49EE-881C-72F2E91A5221}"/>
+    <hyperlink ref="M4" r:id="rId4" xr:uid="{7060CEC9-5B05-4517-94B1-A25E1387F007}"/>
+    <hyperlink ref="H3:H4" r:id="rId5" display="https://www.linkedin.com/Riya" xr:uid="{4655DA96-560C-4320-8868-5A5B48A6AF53}"/>
+    <hyperlink ref="M5" r:id="rId6" xr:uid="{F04495E7-7D15-43B4-9835-4C834961BFF9}"/>
+    <hyperlink ref="H5" r:id="rId7" xr:uid="{D9D52848-1F3E-43E8-AFCE-B3EB6F2859B7}"/>
+    <hyperlink ref="M6" r:id="rId8" xr:uid="{73D22A5E-E713-49C5-98F0-59006700DC1E}"/>
+    <hyperlink ref="H6" r:id="rId9" xr:uid="{612223B7-09ED-4F6E-BF98-199C7F889A4F}"/>
+    <hyperlink ref="M7" r:id="rId10" xr:uid="{B28F044C-C703-465D-ACB6-229DB28CC16E}"/>
+    <hyperlink ref="M8" r:id="rId11" xr:uid="{3F96FC15-111A-4960-8BC9-13434DA66FA2}"/>
+    <hyperlink ref="M9" r:id="rId12" xr:uid="{FA843723-F6D8-4B35-A7A6-BE81158240B9}"/>
+    <hyperlink ref="M10" r:id="rId13" xr:uid="{10CEDCC6-DC7E-4C31-B34B-68669CDA8272}"/>
+    <hyperlink ref="M19" r:id="rId14" xr:uid="{A0BE1B62-7EA3-4C76-9DAB-C0258E5DA16D}"/>
+    <hyperlink ref="H19" r:id="rId15" xr:uid="{9046725B-9384-405B-8D81-80EF228335E5}"/>
+    <hyperlink ref="M18" r:id="rId16" xr:uid="{2B09A2BB-81ED-40BE-97BA-5E5CA838C840}"/>
+    <hyperlink ref="H18" r:id="rId17" xr:uid="{D5152253-593B-4CB7-AD01-150F7CEAA55F}"/>
+    <hyperlink ref="H20" r:id="rId18" xr:uid="{18AB9E42-5763-4BE0-8A1A-EF127C593C61}"/>
+    <hyperlink ref="O20" r:id="rId19" xr:uid="{3811F4B1-2A13-428D-AE7C-78653F92C81E}"/>
+    <hyperlink ref="M21" r:id="rId20" xr:uid="{80C48906-FF0A-4D3F-9CC1-BF3387213AAD}"/>
+    <hyperlink ref="M22" r:id="rId21" xr:uid="{C27C6FB0-96DC-4D41-80EF-55818CF88748}"/>
+    <hyperlink ref="H22" r:id="rId22" xr:uid="{084BF7EF-0485-4C27-A65A-65CE4FCB43AC}"/>
+    <hyperlink ref="M20" r:id="rId23" xr:uid="{0264487A-EC9E-4AC2-A98A-BEB64091B0E6}"/>
+    <hyperlink ref="H21" r:id="rId24" xr:uid="{1F685D3A-6BDE-49D1-831B-4B684593642D}"/>
+    <hyperlink ref="H24" r:id="rId25" xr:uid="{26C0569C-143C-4159-AAFB-F6F5DB1B825A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix merge conflicts for manage program module
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData/TestData.xlsx
+++ b/src/test/resources/ExcelTestData/TestData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Priyanka Numpy Ninja docs and Projects\LMS_Team15_Apr2024\LMS-Hackathon-Team-15\src\test\resources\ExcelTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kundu\git\LMS-Hackathon-temp-branch\LMS-Hackathon-Team-15\src\test\resources\ExcelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BE8B8C-6451-4F99-BFCC-AEC8FF14B820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5F3E16-0EF6-48FA-A3AD-12B41AED11A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17280" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
     <sheet name="LoginPage" sheetId="2" r:id="rId2"/>
     <sheet name="UserPage_Edit" sheetId="3" r:id="rId3"/>
+    <sheet name="ProgramPage" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="156">
   <si>
     <t>Please login to LMS application</t>
   </si>
@@ -471,6 +472,33 @@
   </si>
   <si>
     <t>optional fields added</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
+    <t>ProgramDescription</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>EditProgramName</t>
+  </si>
+  <si>
+    <t>EditProgramDescription</t>
+  </si>
+  <si>
+    <t>RubySJC1234</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>RDBMS123</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -839,30 +867,30 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="55.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="2"/>
+    <col min="12" max="12" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="55.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -918,7 +946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -926,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -935,7 +963,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -943,7 +971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -951,7 +979,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -959,7 +987,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -968,7 +996,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -977,7 +1005,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -986,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -994,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1002,7 +1030,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
@@ -1010,7 +1038,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1018,7 +1046,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -1026,7 +1054,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -1034,7 +1062,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -1042,7 +1070,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -1050,7 +1078,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1075,15 +1103,15 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1098,7 +1126,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1111,7 +1139,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1122,7 +1150,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1133,7 +1161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1141,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1152,7 +1180,7 @@
         <v>1234446</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1166,30 +1194,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788AA9AD-10DC-4CF5-9D53-5F59AF9B065B}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1239,7 +1267,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>116</v>
       </c>
@@ -1261,7 +1289,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
@@ -1309,7 +1337,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>58</v>
       </c>
@@ -1357,7 +1385,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>76</v>
       </c>
@@ -1405,7 +1433,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
@@ -1453,7 +1481,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>78</v>
       </c>
@@ -1501,7 +1529,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>79</v>
       </c>
@@ -1549,7 +1577,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>60</v>
       </c>
@@ -1597,7 +1625,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
@@ -1645,7 +1673,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
@@ -1693,7 +1721,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>81</v>
       </c>
@@ -1741,7 +1769,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
@@ -1789,7 +1817,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>83</v>
       </c>
@@ -1837,7 +1865,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>107</v>
       </c>
@@ -1885,7 +1913,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>117</v>
       </c>
@@ -1933,7 +1961,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>142</v>
       </c>
@@ -1981,7 +2009,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>132</v>
       </c>
@@ -2029,7 +2057,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>133</v>
       </c>
@@ -2077,7 +2105,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>134</v>
       </c>
@@ -2125,7 +2153,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>135</v>
       </c>
@@ -2173,7 +2201,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>137</v>
       </c>
@@ -2221,7 +2249,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>130</v>
       </c>
@@ -2252,7 +2280,7 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>140</v>
       </c>
@@ -2297,7 +2325,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>143</v>
       </c>
@@ -2350,4 +2378,60 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A11C47B-6836-4CA0-BFB1-AC15A680A80F}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>